<commit_message>
auto tab for category and date buttons, filepath fix for lucille transactions.
</commit_message>
<xml_diff>
--- a/LM Sheet (by Juan Alduey).xlsx
+++ b/LM Sheet (by Juan Alduey).xlsx
@@ -5,12 +5,12 @@
   <workbookPr date1904="1" showInkAnnotation="0" codeName="ThisWorkbook" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ceciliametheny/Desktop/Cecilia Numbers with Macros/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ceciliametheny/repos/ceciliametheny/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{31B30BF6-57B1-DD4C-80B7-C528F97772DD}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{129DFE6E-BA40-774C-8365-35DEAAFBFBB0}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16420" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16340" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Income" sheetId="1" r:id="rId1"/>
@@ -599,8 +599,8 @@
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="Income"/>
+      <sheetName val="Expenses"/>
       <sheetName val="Categories and Stats"/>
-      <sheetName val="Expenses"/>
       <sheetName val="DebitCredit Card Bank Acct Data"/>
       <sheetName val="Petty Cash Envelope"/>
       <sheetName val="TimeLog"/>
@@ -610,7 +610,8 @@
     </definedNames>
     <sheetDataSet>
       <sheetData sheetId="0"/>
-      <sheetData sheetId="1">
+      <sheetData sheetId="1"/>
+      <sheetData sheetId="2">
         <row r="2">
           <cell r="G2" t="str">
             <v>Rent</v>
@@ -887,7 +888,6 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="2"/>
       <sheetData sheetId="3"/>
       <sheetData sheetId="4"/>
       <sheetData sheetId="5"/>
@@ -1219,9 +1219,9 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E5" sqref="E5"/>
+      <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -1322,9 +1322,9 @@
   <sheetPr codeName="Sheet1" filterMode="1"/>
   <dimension ref="A1:F59"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A42" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A59" sqref="A59"/>
+      <selection pane="bottomLeft" activeCell="A60" sqref="A60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -2168,10 +2168,10 @@
   </autoFilter>
   <phoneticPr fontId="2" type="noConversion"/>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B43:B46 B55 B1:B41 B60:B1048576" xr:uid="{00000000-0002-0000-0100-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B43:B46 B55 B1:B41 B61:B1048576" xr:uid="{00000000-0002-0000-0100-000000000000}">
       <formula1>expense</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B47:B54 B42 B56:B59" xr:uid="{05177A31-2436-494B-9BEE-6D517E3064DB}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B47:B54 B42 B56:B60" xr:uid="{05177A31-2436-494B-9BEE-6D517E3064DB}">
       <formula1>expenses</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
made separate workbook for timelog and petty cash
</commit_message>
<xml_diff>
--- a/LM Sheet (by Juan Alduey).xlsx
+++ b/LM Sheet (by Juan Alduey).xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10319"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10319"/>
   <workbookPr date1904="1" showInkAnnotation="0" codeName="ThisWorkbook" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ceciliametheny/repos/ceciliametheny/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{129DFE6E-BA40-774C-8365-35DEAAFBFBB0}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{28639C57-1C9D-7C4F-AB17-AAC08A3A9A2A}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16340" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
     <externalReference r:id="rId4"/>
   </externalReferences>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Expense!$A$1:$D$57</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Expense!$A$1:$D$59</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Income!$A$1:$D$1</definedName>
     <definedName name="expense">Categories!$F$2:$F$15</definedName>
     <definedName name="expenses">'[1]Categories and Stats'!$G$2:$G$56</definedName>
@@ -604,6 +604,7 @@
       <sheetName val="DebitCredit Card Bank Acct Data"/>
       <sheetName val="Petty Cash Envelope"/>
       <sheetName val="TimeLog"/>
+      <sheetName val="CM Sheet (by Juan Alduey)"/>
     </sheetNames>
     <definedNames>
       <definedName name="cmExp"/>
@@ -889,8 +890,9 @@
         </row>
       </sheetData>
       <sheetData sheetId="3"/>
-      <sheetData sheetId="4"/>
-      <sheetData sheetId="5"/>
+      <sheetData sheetId="4" refreshError="1"/>
+      <sheetData sheetId="5" refreshError="1"/>
+      <sheetData sheetId="6" refreshError="1"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -1221,7 +1223,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
+      <selection pane="bottomLeft" activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -1319,12 +1321,12 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <sheetPr codeName="Sheet1" filterMode="1"/>
+  <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:F59"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A42" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A60" sqref="A60"/>
+      <pane ySplit="1" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A59" sqref="A59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -1349,7 +1351,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="2" spans="1:4" hidden="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A2" s="3">
         <v>41646</v>
       </c>
@@ -1360,7 +1362,7 @@
         <v>11.49</v>
       </c>
     </row>
-    <row r="3" spans="1:4" hidden="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A3" s="3">
         <v>41647</v>
       </c>
@@ -1371,7 +1373,7 @@
         <v>8.2899999999999991</v>
       </c>
     </row>
-    <row r="4" spans="1:4" hidden="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A4" s="3">
         <v>41647</v>
       </c>
@@ -1385,7 +1387,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="5" spans="1:4" hidden="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A5" s="3">
         <v>41654</v>
       </c>
@@ -1399,7 +1401,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="6" spans="1:4" hidden="1" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A6" s="3">
         <v>41657</v>
       </c>
@@ -1410,7 +1412,7 @@
         <v>2790</v>
       </c>
     </row>
-    <row r="7" spans="1:4" hidden="1" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A7" s="3">
         <v>41658</v>
       </c>
@@ -1424,7 +1426,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="8" spans="1:4" hidden="1" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A8" s="3">
         <v>41660</v>
       </c>
@@ -1438,7 +1440,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="9" spans="1:4" hidden="1" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A9" s="3">
         <v>41663</v>
       </c>
@@ -1452,7 +1454,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="10" spans="1:4" hidden="1" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A10" s="3">
         <v>41664</v>
       </c>
@@ -1466,7 +1468,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="11" spans="1:4" hidden="1" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A11" s="3">
         <v>41665</v>
       </c>
@@ -1480,7 +1482,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="1:4" hidden="1" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A12" s="3">
         <v>41667</v>
       </c>
@@ -1491,7 +1493,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="13" spans="1:4" hidden="1" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A13" s="3">
         <v>41670</v>
       </c>
@@ -1505,91 +1507,91 @@
         <v>52</v>
       </c>
     </row>
-    <row r="14" spans="1:4" hidden="1" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A14" s="3">
-        <v>41677</v>
+        <v>41675</v>
       </c>
       <c r="B14" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="C14" s="7">
-        <v>19.899999999999999</v>
+        <v>1000</v>
       </c>
       <c r="D14" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" hidden="1" x14ac:dyDescent="0.15">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A15" s="3">
         <v>41677</v>
       </c>
       <c r="B15" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="C15" s="7">
-        <v>93.51</v>
+        <v>19.899999999999999</v>
       </c>
       <c r="D15" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" hidden="1" x14ac:dyDescent="0.15">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A16" s="3">
-        <v>41679</v>
+        <v>41677</v>
       </c>
       <c r="B16" t="s">
         <v>60</v>
       </c>
       <c r="C16" s="7">
-        <v>18.5</v>
+        <v>93.51</v>
       </c>
       <c r="D16" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" hidden="1" x14ac:dyDescent="0.15">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A17" s="3">
         <v>41679</v>
       </c>
       <c r="B17" t="s">
-        <v>72</v>
+        <v>60</v>
       </c>
       <c r="C17" s="7">
-        <v>19.23</v>
+        <v>18.5</v>
       </c>
       <c r="D17" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" hidden="1" x14ac:dyDescent="0.15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A18" s="3">
         <v>41679</v>
       </c>
       <c r="B18" t="s">
-        <v>60</v>
+        <v>72</v>
       </c>
       <c r="C18" s="7">
-        <v>181.82</v>
+        <v>19.23</v>
       </c>
       <c r="D18" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" hidden="1" x14ac:dyDescent="0.15">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A19" s="3">
-        <v>41680</v>
+        <v>41679</v>
       </c>
       <c r="B19" t="s">
         <v>60</v>
       </c>
       <c r="C19" s="7">
-        <v>17.29</v>
+        <v>181.82</v>
       </c>
       <c r="D19" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" hidden="1" x14ac:dyDescent="0.15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A20" s="3">
         <v>41680</v>
       </c>
@@ -1597,69 +1599,69 @@
         <v>60</v>
       </c>
       <c r="C20" s="7">
-        <v>19.059999999999999</v>
+        <v>17.29</v>
       </c>
       <c r="D20" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" hidden="1" x14ac:dyDescent="0.15">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A21" s="3">
         <v>41680</v>
       </c>
       <c r="B21" t="s">
+        <v>60</v>
+      </c>
+      <c r="C21" s="7">
+        <v>19.059999999999999</v>
+      </c>
+      <c r="D21" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A22" s="3">
+        <v>41680</v>
+      </c>
+      <c r="B22" t="s">
         <v>65</v>
       </c>
-      <c r="C21" s="7">
+      <c r="C22" s="7">
         <v>77.52</v>
       </c>
-      <c r="D21" t="s">
+      <c r="D22" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="22" spans="1:4" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A22" s="3">
-        <v>41681</v>
-      </c>
-      <c r="B22" t="s">
-        <v>2</v>
-      </c>
-      <c r="C22" s="7">
-        <v>23</v>
-      </c>
-      <c r="D22" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" hidden="1" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A23" s="3">
         <v>41681</v>
       </c>
       <c r="B23" t="s">
-        <v>60</v>
+        <v>2</v>
       </c>
       <c r="C23" s="7">
-        <v>48.38</v>
+        <v>23</v>
       </c>
       <c r="D23" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" hidden="1" x14ac:dyDescent="0.15">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A24" s="3">
         <v>41681</v>
       </c>
-      <c r="B24" s="12" t="s">
-        <v>57</v>
+      <c r="B24" t="s">
+        <v>60</v>
       </c>
       <c r="C24" s="7">
-        <v>28.38</v>
+        <v>48.38</v>
       </c>
       <c r="D24" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" hidden="1" x14ac:dyDescent="0.15">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A25" s="3">
         <v>41681</v>
       </c>
@@ -1670,80 +1672,80 @@
         <v>28.38</v>
       </c>
       <c r="D25" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A26" s="3">
+        <v>41681</v>
+      </c>
+      <c r="B26" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="C26" s="7">
+        <v>28.38</v>
+      </c>
+      <c r="D26" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="26" spans="1:4" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A26" s="3">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A27" s="3">
         <v>41682</v>
       </c>
-      <c r="B26" t="s">
+      <c r="B27" t="s">
         <v>63</v>
       </c>
-      <c r="C26" s="7">
+      <c r="C27" s="7">
         <v>61.7</v>
       </c>
-      <c r="D26" t="s">
+      <c r="D27" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="27" spans="1:4" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A27" s="3">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A28" s="3">
         <v>41683</v>
       </c>
-      <c r="B27" t="s">
+      <c r="B28" t="s">
         <v>60</v>
       </c>
-      <c r="C27" s="7">
+      <c r="C28" s="7">
         <v>96.57</v>
       </c>
-      <c r="D27" t="s">
+      <c r="D28" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="28" spans="1:4" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A28" s="3">
-        <v>41691</v>
-      </c>
-      <c r="B28" t="s">
-        <v>48</v>
-      </c>
-      <c r="C28" s="7">
-        <v>400</v>
-      </c>
-      <c r="D28" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" hidden="1" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A29" s="3">
         <v>41691</v>
       </c>
       <c r="B29" t="s">
-        <v>21</v>
+        <v>48</v>
       </c>
       <c r="C29" s="7">
-        <v>2790</v>
+        <v>400</v>
       </c>
       <c r="D29" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" hidden="1" x14ac:dyDescent="0.15">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A30" s="3">
         <v>41691</v>
       </c>
       <c r="B30" t="s">
-        <v>52</v>
+        <v>21</v>
       </c>
       <c r="C30" s="7">
         <v>2790</v>
       </c>
       <c r="D30" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" hidden="1" x14ac:dyDescent="0.15">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A31" s="3">
         <v>41691</v>
       </c>
@@ -1754,88 +1756,88 @@
         <v>2790</v>
       </c>
       <c r="D31" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A32" s="3">
+        <v>41691</v>
+      </c>
+      <c r="B32" t="s">
+        <v>52</v>
+      </c>
+      <c r="C32" s="7">
+        <v>2790</v>
+      </c>
+      <c r="D32" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="32" spans="1:4" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A32" s="3">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A33" s="3">
         <v>41692</v>
       </c>
-      <c r="B32" t="s">
+      <c r="B33" t="s">
         <v>10</v>
       </c>
-      <c r="C32" s="7">
+      <c r="C33" s="7">
         <v>200</v>
       </c>
     </row>
-    <row r="33" spans="1:4" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A33" s="3">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A34" s="3">
         <v>41695</v>
       </c>
-      <c r="B33" t="s">
+      <c r="B34" t="s">
         <v>59</v>
       </c>
-      <c r="C33" s="7">
+      <c r="C34" s="7">
         <v>3000</v>
       </c>
     </row>
-    <row r="34" spans="1:4" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A34" s="3">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A35" s="3">
         <v>41698</v>
       </c>
-      <c r="B34" t="s">
+      <c r="B35" t="s">
         <v>57</v>
       </c>
-      <c r="C34" s="7">
+      <c r="C35" s="7">
         <v>1000</v>
       </c>
-      <c r="D34" s="12" t="s">
+      <c r="D35" s="12" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="35" spans="1:4" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A35" s="3">
-        <v>41700</v>
-      </c>
-      <c r="B35" t="s">
-        <v>60</v>
-      </c>
-      <c r="C35" s="7">
-        <v>77.31</v>
-      </c>
-      <c r="D35" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" hidden="1" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A36" s="3">
         <v>41700</v>
       </c>
       <c r="B36" t="s">
+        <v>60</v>
+      </c>
+      <c r="C36" s="7">
+        <v>77.31</v>
+      </c>
+      <c r="D36" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A37" s="3">
+        <v>41700</v>
+      </c>
+      <c r="B37" t="s">
         <v>5</v>
       </c>
-      <c r="C36" s="7">
+      <c r="C37" s="7">
         <v>79.19</v>
       </c>
-      <c r="D36" t="s">
+      <c r="D37" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="37" spans="1:4" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A37" s="3">
-        <v>41701</v>
-      </c>
-      <c r="B37" s="12" t="s">
-        <v>57</v>
-      </c>
-      <c r="C37" s="7">
-        <v>12.36</v>
-      </c>
-      <c r="D37" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" hidden="1" x14ac:dyDescent="0.15">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A38" s="3">
         <v>41701</v>
       </c>
@@ -1843,27 +1845,27 @@
         <v>57</v>
       </c>
       <c r="C38" s="7">
+        <v>12.36</v>
+      </c>
+      <c r="D38" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A39" s="3">
+        <v>41701</v>
+      </c>
+      <c r="B39" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="C39" s="7">
         <v>12.96</v>
       </c>
-      <c r="D38" t="s">
+      <c r="D39" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="39" spans="1:4" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A39" s="3">
-        <v>41702</v>
-      </c>
-      <c r="B39" t="s">
-        <v>60</v>
-      </c>
-      <c r="C39" s="7">
-        <v>6.99</v>
-      </c>
-      <c r="D39" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" hidden="1" x14ac:dyDescent="0.15">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A40" s="3">
         <v>41702</v>
       </c>
@@ -1874,252 +1876,252 @@
         <v>6.99</v>
       </c>
       <c r="D40" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" hidden="1" x14ac:dyDescent="0.15">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A41" s="3">
         <v>41702</v>
       </c>
       <c r="B41" t="s">
-        <v>11</v>
+        <v>60</v>
       </c>
       <c r="C41" s="7">
-        <v>102.5</v>
+        <v>6.99</v>
       </c>
       <c r="D41" t="s">
-        <v>18</v>
+        <v>62</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A42" s="3">
+        <v>41702</v>
+      </c>
+      <c r="B42" t="s">
+        <v>11</v>
+      </c>
+      <c r="C42" s="7">
+        <v>102.5</v>
+      </c>
+      <c r="D42" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A43" s="3">
         <v>41703</v>
       </c>
-      <c r="B42" t="s">
+      <c r="B43" t="s">
         <v>57</v>
       </c>
-      <c r="C42" s="7">
+      <c r="C43" s="7">
         <v>1000</v>
       </c>
-      <c r="D42" s="12" t="s">
+      <c r="D43" s="12" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="43" spans="1:4" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A43" s="3">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A44" s="3">
         <v>41706</v>
       </c>
-      <c r="B43" t="s">
+      <c r="B44" t="s">
         <v>11</v>
       </c>
-      <c r="C43" s="7">
+      <c r="C44" s="7">
         <v>2252</v>
       </c>
-      <c r="D43" t="s">
+      <c r="D44" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="44" spans="1:4" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A44" s="3">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A45" s="3">
+        <v>41706</v>
+      </c>
+      <c r="B45" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="C45" s="7">
+        <v>2252</v>
+      </c>
+      <c r="D45" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A46" s="3">
         <v>41707</v>
       </c>
-      <c r="B44" t="s">
+      <c r="B46" t="s">
         <v>57</v>
       </c>
-      <c r="C44" s="7">
+      <c r="C46" s="7">
         <v>28.29</v>
       </c>
-      <c r="D44" t="s">
+      <c r="D46" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="45" spans="1:4" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A45" s="3">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A47" s="3">
         <v>41708</v>
       </c>
-      <c r="B45" t="s">
+      <c r="B47" t="s">
         <v>16</v>
       </c>
-      <c r="C45" s="7">
+      <c r="C47" s="7">
         <v>15.98</v>
       </c>
-      <c r="D45" t="s">
+      <c r="D47" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="46" spans="1:4" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A46" s="3">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A48" s="3">
         <v>41710</v>
       </c>
-      <c r="B46" t="s">
+      <c r="B48" t="s">
         <v>29</v>
       </c>
-      <c r="C46" s="7">
+      <c r="C48" s="7">
         <v>250</v>
       </c>
-      <c r="D46" s="12" t="s">
+      <c r="D48" s="12" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="47" spans="1:4" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A47" s="3">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A49" s="3">
         <v>41710</v>
       </c>
-      <c r="B47" t="s">
+      <c r="B49" t="s">
         <v>40</v>
       </c>
-      <c r="C47" s="7">
+      <c r="C49" s="7">
         <v>650</v>
       </c>
-      <c r="D47" s="12" t="s">
+      <c r="D49" s="12" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="48" spans="1:4" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A48" s="3">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A50" s="3">
         <v>41714</v>
-      </c>
-      <c r="B48" s="12" t="s">
-        <v>57</v>
-      </c>
-      <c r="C48" s="7">
-        <v>133.32</v>
-      </c>
-      <c r="D48" s="12" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="49" spans="1:6" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A49" s="3">
-        <v>41719</v>
-      </c>
-      <c r="B49" t="s">
-        <v>32</v>
-      </c>
-      <c r="C49" s="7">
-        <v>400</v>
-      </c>
-      <c r="D49" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="50" spans="1:6" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A50" s="3">
-        <v>41719</v>
       </c>
       <c r="B50" s="12" t="s">
         <v>57</v>
       </c>
       <c r="C50" s="7">
-        <v>39.29</v>
-      </c>
-      <c r="D50" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="51" spans="1:6" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A51" s="13">
-        <v>41721</v>
-      </c>
-      <c r="B51" s="12" t="s">
-        <v>57</v>
+        <v>133.32</v>
+      </c>
+      <c r="D50" s="12" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A51" s="3">
+        <v>41719</v>
+      </c>
+      <c r="B51" t="s">
+        <v>32</v>
       </c>
       <c r="C51" s="7">
-        <v>129.56</v>
-      </c>
-      <c r="D51" s="12" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="52" spans="1:6" hidden="1" x14ac:dyDescent="0.15">
+        <v>400</v>
+      </c>
+      <c r="D51" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A52" s="3">
-        <v>41729</v>
+        <v>41719</v>
       </c>
       <c r="B52" s="12" t="s">
         <v>57</v>
       </c>
       <c r="C52" s="7">
-        <v>1000</v>
+        <v>39.29</v>
       </c>
       <c r="D52" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="E52" s="12" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="53" spans="1:6" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A53" s="3">
-        <v>41730</v>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A53" s="13">
+        <v>41721</v>
       </c>
       <c r="B53" s="12" t="s">
         <v>57</v>
       </c>
       <c r="C53" s="7">
-        <v>153.13</v>
-      </c>
-      <c r="D53" t="s">
-        <v>83</v>
+        <v>129.56</v>
+      </c>
+      <c r="D53" s="12" t="s">
+        <v>75</v>
       </c>
       <c r="E53" s="12"/>
       <c r="F53" s="12" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="54" spans="1:6" hidden="1" x14ac:dyDescent="0.15">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A54" s="3">
-        <v>41706</v>
-      </c>
-      <c r="B54" s="12" t="s">
+        <v>41726</v>
+      </c>
+      <c r="B54" t="s">
         <v>57</v>
       </c>
       <c r="C54" s="7">
-        <v>2252</v>
+        <v>346.22</v>
       </c>
       <c r="D54" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="55" spans="1:6" hidden="1" x14ac:dyDescent="0.15">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A55" s="3">
-        <v>41730</v>
+        <v>41729</v>
       </c>
       <c r="B55" s="12" t="s">
         <v>57</v>
       </c>
       <c r="C55" s="7">
-        <v>139.5</v>
-      </c>
-      <c r="D55" s="12" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="56" spans="1:6" hidden="1" x14ac:dyDescent="0.15">
+        <v>1000</v>
+      </c>
+      <c r="D55" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A56" s="3">
-        <v>41731</v>
+        <v>41730</v>
       </c>
       <c r="B56" s="12" t="s">
         <v>57</v>
       </c>
       <c r="C56" s="7">
-        <v>1000</v>
+        <v>153.13</v>
       </c>
       <c r="D56" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="57" spans="1:6" hidden="1" x14ac:dyDescent="0.15">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A57" s="3">
-        <v>41675</v>
-      </c>
-      <c r="B57" t="s">
+        <v>41730</v>
+      </c>
+      <c r="B57" s="12" t="s">
         <v>57</v>
       </c>
       <c r="C57" s="7">
-        <v>1000</v>
-      </c>
-      <c r="D57" t="s">
-        <v>81</v>
+        <v>139.5</v>
+      </c>
+      <c r="D57" s="12" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.15">
@@ -2132,46 +2134,36 @@
       <c r="C58" s="7">
         <v>1000</v>
       </c>
-      <c r="D58" s="12" t="s">
-        <v>89</v>
+      <c r="D58" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A59" s="3">
-        <v>41726</v>
-      </c>
-      <c r="B59" t="s">
+        <v>41731</v>
+      </c>
+      <c r="B59" s="12" t="s">
         <v>57</v>
       </c>
       <c r="C59" s="7">
-        <v>346.22</v>
-      </c>
-      <c r="D59" t="s">
-        <v>90</v>
+        <v>1000</v>
+      </c>
+      <c r="D59" s="12" t="s">
+        <v>89</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:D57" xr:uid="{00000000-0009-0000-0000-000001000000}">
-    <filterColumn colId="1">
-      <filters>
-        <filter val="Cecilia Metheny"/>
-      </filters>
-    </filterColumn>
-    <filterColumn colId="3">
-      <filters>
-        <filter val="for Juan Alduey"/>
-      </filters>
-    </filterColumn>
-    <sortState ref="A42:D58">
-      <sortCondition ref="D1:D58"/>
+  <autoFilter ref="A1:D59" xr:uid="{00000000-0009-0000-0000-000001000000}">
+    <sortState ref="A2:D59">
+      <sortCondition ref="A1:A59"/>
     </sortState>
   </autoFilter>
   <phoneticPr fontId="2" type="noConversion"/>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B43:B46 B55 B1:B41 B61:B1048576" xr:uid="{00000000-0002-0000-0100-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B43:B46 B55 B1:B41 B60:B1048576" xr:uid="{00000000-0002-0000-0100-000000000000}">
       <formula1>expense</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B47:B54 B42 B56:B60" xr:uid="{05177A31-2436-494B-9BEE-6D517E3064DB}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B47:B54 B42 B56:B59" xr:uid="{05177A31-2436-494B-9BEE-6D517E3064DB}">
       <formula1>expenses</formula1>
     </dataValidation>
   </dataValidations>
@@ -2414,7 +2406,7 @@
       </c>
       <c r="G15" s="8">
         <f>SUMIFS(ExpensesAmtLog, ExpensesCatLog, F15, ExpensesDateLog, "&gt;="&amp;TEXT($J$2, "mm-dd-yyyy"), ExpensesDateLog, "&lt;="&amp;TEXT($K$2, "mm-dd-yyyy"))</f>
-        <v>10690.249999999998</v>
+        <v>10690.25</v>
       </c>
     </row>
     <row r="16" spans="2:11" x14ac:dyDescent="0.15">

</xml_diff>

<commit_message>
Clear filter buttons for LM sheet. New '3 month average' tab on cm sheet.
</commit_message>
<xml_diff>
--- a/LM Sheet (by Juan Alduey).xlsx
+++ b/LM Sheet (by Juan Alduey).xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ceciliametheny/repos/ceciliametheny/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{28639C57-1C9D-7C4F-AB17-AAC08A3A9A2A}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{EB630F6F-9073-C24B-8750-19A1B697B34C}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16340" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16340" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Income" sheetId="1" r:id="rId1"/>
@@ -19,10 +19,11 @@
   </sheets>
   <externalReferences>
     <externalReference r:id="rId4"/>
+    <externalReference r:id="rId5"/>
   </externalReferences>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Expense!$A$1:$D$59</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Income!$A$1:$D$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Income!$A$1:$D$5</definedName>
     <definedName name="expense">Categories!$F$2:$F$15</definedName>
     <definedName name="expenses">'[1]Categories and Stats'!$G$2:$G$56</definedName>
     <definedName name="ExpensesAmtLog">Expense!$C:$C</definedName>
@@ -520,7 +521,90 @@
 <formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Button" lockText="1"/>
 </file>
 
+<file path=xl/ctrlProps/ctrlProp2.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Button" lockText="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp3.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Button" lockText="1"/>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor>
+        <xdr:from>
+          <xdr:col>4</xdr:col>
+          <xdr:colOff>266700</xdr:colOff>
+          <xdr:row>0</xdr:row>
+          <xdr:rowOff>101600</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>6</xdr:col>
+          <xdr:colOff>152400</xdr:colOff>
+          <xdr:row>0</xdr:row>
+          <xdr:rowOff>495300</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="2049" name="Button 1" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s2049"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8556D145-660E-7E4F-8CCD-6A9F00A05EF9}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln w="9525">
+              <a:miter lim="800000"/>
+              <a:headEnd/>
+              <a:tailEnd/>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="27432" bIns="18288" anchor="ctr" upright="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr algn="ctr" rtl="0">
+                <a:defRPr sz="1000"/>
+              </a:pPr>
+              <a:r>
+                <a:rPr lang="en-US" sz="1000" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                  <a:solidFill>
+                    <a:srgbClr val="000000"/>
+                  </a:solidFill>
+                  <a:latin typeface="Verdana" charset="0"/>
+                  <a:ea typeface="Verdana" charset="0"/>
+                  <a:cs typeface="Verdana" charset="0"/>
+                </a:rPr>
+                <a:t>Clear Filters</a:t>
+              </a:r>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+        <xdr:clientData fPrintsWithSheet="0"/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
@@ -591,6 +675,76 @@
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor>
+        <xdr:from>
+          <xdr:col>4</xdr:col>
+          <xdr:colOff>279400</xdr:colOff>
+          <xdr:row>0</xdr:row>
+          <xdr:rowOff>114300</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>6</xdr:col>
+          <xdr:colOff>165100</xdr:colOff>
+          <xdr:row>0</xdr:row>
+          <xdr:rowOff>482600</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="1026" name="Button 2" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s1026"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EB3B128A-DEF4-7445-998C-A537DA7C5176}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln w="9525">
+              <a:miter lim="800000"/>
+              <a:headEnd/>
+              <a:tailEnd/>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="27432" bIns="18288" anchor="ctr" upright="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr algn="ctr" rtl="0">
+                <a:defRPr sz="1000"/>
+              </a:pPr>
+              <a:r>
+                <a:rPr lang="en-US" sz="1000" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                  <a:solidFill>
+                    <a:srgbClr val="000000"/>
+                  </a:solidFill>
+                  <a:latin typeface="Verdana" charset="0"/>
+                  <a:ea typeface="Verdana" charset="0"/>
+                  <a:cs typeface="Verdana" charset="0"/>
+                </a:rPr>
+                <a:t>Clear Filters</a:t>
+              </a:r>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+        <xdr:clientData fPrintsWithSheet="0"/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
 </xdr:wsDr>
 </file>
 
@@ -893,6 +1047,28 @@
       <sheetData sheetId="4" refreshError="1"/>
       <sheetData sheetId="5" refreshError="1"/>
       <sheetData sheetId="6" refreshError="1"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
+</file>
+
+<file path=xl/externalLinks/externalLink2.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="Income"/>
+      <sheetName val="Expenses"/>
+      <sheetName val="Categories and Stats"/>
+      <sheetName val="DebitCredit Card Bank Acct Data"/>
+    </sheetNames>
+    <definedNames>
+      <definedName name="ClearFilters.ClearFilters"/>
+    </definedNames>
+    <sheetDataSet>
+      <sheetData sheetId="0"/>
+      <sheetData sheetId="1"/>
+      <sheetData sheetId="2"/>
+      <sheetData sheetId="3"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -1217,13 +1393,13 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E5" sqref="E5"/>
+      <selection pane="bottomLeft" activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -1232,7 +1408,7 @@
     <col min="3" max="3" width="10.6640625" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="28" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:4" ht="47" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="2" t="s">
         <v>42</v>
       </c>
@@ -1303,7 +1479,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:D1" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:D5" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <phoneticPr fontId="2" type="noConversion"/>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B1048576" xr:uid="{00000000-0002-0000-0000-000000000000}">
@@ -1311,6 +1487,36 @@
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <drawing r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x14">
+      <controls>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="2049" r:id="rId3" name="Button 1">
+              <controlPr defaultSize="0" print="0" autoFill="0" autoPict="0" macro="[2]!ClearFilters.ClearFilters">
+                <anchor moveWithCells="1" sizeWithCells="1">
+                  <from>
+                    <xdr:col>4</xdr:col>
+                    <xdr:colOff>266700</xdr:colOff>
+                    <xdr:row>0</xdr:row>
+                    <xdr:rowOff>101600</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>6</xdr:col>
+                    <xdr:colOff>152400</xdr:colOff>
+                    <xdr:row>0</xdr:row>
+                    <xdr:rowOff>495300</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+      </controls>
+    </mc:Choice>
+  </mc:AlternateContent>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -1324,9 +1530,9 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:F59"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A59" sqref="A59"/>
+      <selection pane="bottomLeft" activeCell="F66" sqref="F66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -2153,11 +2359,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:D59" xr:uid="{00000000-0009-0000-0000-000001000000}">
-    <sortState ref="A2:D59">
-      <sortCondition ref="A1:A59"/>
-    </sortState>
-  </autoFilter>
+  <autoFilter ref="A1:D59" xr:uid="{00000000-0009-0000-0000-000001000000}"/>
   <phoneticPr fontId="2" type="noConversion"/>
   <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B43:B46 B55 B1:B41 B60:B1048576" xr:uid="{00000000-0002-0000-0100-000000000000}">
@@ -2195,6 +2397,28 @@
             </control>
           </mc:Choice>
         </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="1026" r:id="rId4" name="Button 2">
+              <controlPr defaultSize="0" print="0" autoFill="0" autoPict="0" macro="[2]!ClearFilters.ClearFilters">
+                <anchor moveWithCells="1" sizeWithCells="1">
+                  <from>
+                    <xdr:col>4</xdr:col>
+                    <xdr:colOff>279400</xdr:colOff>
+                    <xdr:row>0</xdr:row>
+                    <xdr:rowOff>114300</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>6</xdr:col>
+                    <xdr:colOff>165100</xdr:colOff>
+                    <xdr:row>0</xdr:row>
+                    <xdr:rowOff>482600</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
       </controls>
     </mc:Choice>
   </mc:AlternateContent>

</xml_diff>

<commit_message>
fixed category and date buttons to prompt for blank cell when selection is not blank
</commit_message>
<xml_diff>
--- a/LM Sheet (by Juan Alduey).xlsx
+++ b/LM Sheet (by Juan Alduey).xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ceciliametheny/repos/ceciliametheny/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{0CE9718D-24D4-2B44-A249-DFD2F7BC30DB}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{CEE04A7D-2A24-2548-BEC3-E0ACD42797AD}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="540" windowWidth="28800" windowHeight="16340" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="94">
   <si>
     <t>for Jewlery repair</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -386,6 +386,12 @@
   </si>
   <si>
     <t>income/G&amp;E</t>
+  </si>
+  <si>
+    <t xml:space="preserve">for  - </t>
+  </si>
+  <si>
+    <t>for Food Out - 53B - 4896</t>
   </si>
 </sst>
 </file>
@@ -764,6 +770,7 @@
       <sheetName val="3 Month Average"/>
     </sheetNames>
     <definedNames>
+      <definedName name="ClearFilters.ClearFilters"/>
       <definedName name="cmExp"/>
     </definedNames>
     <sheetDataSet>
@@ -1378,7 +1385,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="Q17" sqref="Q17"/>
+      <selection pane="bottomLeft" activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -1474,7 +1481,7 @@
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
             <control shapeId="2049" r:id="rId3" name="Button 1">
-              <controlPr defaultSize="0" print="0" autoFill="0" autoPict="0">
+              <controlPr defaultSize="0" print="0" autoFill="0" autoPict="0" macro="[1]!ClearFilters.ClearFilters">
                 <anchor moveWithCells="1" sizeWithCells="1">
                   <from>
                     <xdr:col>4</xdr:col>
@@ -1510,8 +1517,8 @@
   <dimension ref="A1:F62"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A44" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D60" sqref="D60"/>
+      <pane ySplit="1" topLeftCell="A51" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A62" sqref="A62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -2338,23 +2345,59 @@
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="B60" s="12"/>
+      <c r="A60" s="3">
+        <v>41754</v>
+      </c>
+      <c r="B60" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="C60" s="7">
+        <v>35</v>
+      </c>
+      <c r="D60" t="s">
+        <v>92</v>
+      </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="B61" s="12"/>
+      <c r="A61" s="3">
+        <v>41754</v>
+      </c>
+      <c r="B61" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="C61" s="7">
+        <v>35</v>
+      </c>
+      <c r="D61" t="s">
+        <v>93</v>
+      </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="B62" s="12"/>
+      <c r="A62" s="3">
+        <v>41754</v>
+      </c>
+      <c r="B62" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="C62" s="7">
+        <v>35</v>
+      </c>
+      <c r="D62" t="s">
+        <v>82</v>
+      </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:D59" xr:uid="{00000000-0009-0000-0000-000001000000}"/>
   <phoneticPr fontId="2" type="noConversion"/>
-  <dataValidations count="2">
+  <dataValidations count="3">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B43:B46 B55 B1:B41 B63:B1048576" xr:uid="{00000000-0002-0000-0100-000000000000}">
       <formula1>expense</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B47:B54 B42 B56:B62" xr:uid="{05177A31-2436-494B-9BEE-6D517E3064DB}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B47:B54 B42 B56:B59 B62" xr:uid="{05177A31-2436-494B-9BEE-6D517E3064DB}">
       <formula1>expenses</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B60:B61" xr:uid="{9B6D1881-8074-BF46-88DE-694A6D567B19}">
+      <formula1>income</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -2388,7 +2431,7 @@
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
             <control shapeId="1026" r:id="rId4" name="Button 2">
-              <controlPr defaultSize="0" print="0" autoFill="0" autoPict="0">
+              <controlPr defaultSize="0" print="0" autoFill="0" autoPict="0" macro="[1]!ClearFilters.ClearFilters">
                 <anchor moveWithCells="1" sizeWithCells="1">
                   <from>
                     <xdr:col>4</xdr:col>

</xml_diff>